<commit_message>
Clean some outdated files
</commit_message>
<xml_diff>
--- a/Lab/请假.xlsx
+++ b/Lab/请假.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Sync\JianGuo\Course\Master2\TA\Lab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/webliu/Workspace/2025算法课TA/Lab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7732FA-1DC8-4409-9F0E-5620F0F8F7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8099637-EC04-0C4C-A3F1-214864D27363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1785" yWindow="3315" windowWidth="27360" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1780" yWindow="2360" windowWidth="27360" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,67 +25,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>lab1</t>
+    <t>姓名</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>谢昊霖</t>
-  </si>
-  <si>
-    <t>张庭硕</t>
+    <t>学号</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>黄凯华</t>
-  </si>
-  <si>
-    <t>赵子涵</t>
-  </si>
-  <si>
-    <t>U202311572</t>
-  </si>
-  <si>
-    <t>?</t>
+    <t>请假日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>U202311542</t>
-  </si>
-  <si>
-    <t>U202311538</t>
-  </si>
-  <si>
-    <t>U202311558</t>
-  </si>
-  <si>
-    <t>U202311560</t>
-  </si>
-  <si>
-    <t>郝若松</t>
-  </si>
-  <si>
-    <t>U202311569</t>
-  </si>
-  <si>
-    <t>U202311537</t>
-  </si>
-  <si>
-    <t>U202311580</t>
-  </si>
-  <si>
-    <t>U202311567</t>
-  </si>
-  <si>
-    <t>U202311546</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,11 +79,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -406,98 +361,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
+      <c r="C1" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-    </row>
+    <row r="2" spans="1:3"/>
+    <row r="3" spans="1:3"/>
+    <row r="4" spans="1:3"/>
+    <row r="5" spans="1:3"/>
+    <row r="6" spans="1:3"/>
+    <row r="7" spans="1:3"/>
+    <row r="8" spans="1:3"/>
+    <row r="9" spans="1:3"/>
+    <row r="10" spans="1:3"/>
+    <row r="11" spans="1:3"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>